<commit_message>
Architecture redesigned, implementing instructions
</commit_message>
<xml_diff>
--- a/instruction set.xlsx
+++ b/instruction set.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\desktop\c++\Simple 8-bit CPU emulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5474A5FB-6C39-42EB-8A14-DA7139AFB3B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9A130A-EC46-4780-B624-A0EBE7D3BC23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2895" yWindow="0" windowWidth="22500" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="94">
   <si>
     <t>A</t>
   </si>
@@ -54,21 +54,12 @@
     <t>MOV R, R</t>
   </si>
   <si>
-    <t>MOV R, a8</t>
-  </si>
-  <si>
-    <t>MOV a8, R</t>
-  </si>
-  <si>
     <t>MOV [R], R</t>
   </si>
   <si>
     <t>MOV [R], [R]</t>
   </si>
   <si>
-    <t>MOV [R], a8</t>
-  </si>
-  <si>
     <t>сокращения в мнемониках</t>
   </si>
   <si>
@@ -96,21 +87,12 @@
     <t>8-битный адрес в регистре</t>
   </si>
   <si>
-    <t>MOV a8, d8</t>
-  </si>
-  <si>
     <t>MOV [R], d8</t>
   </si>
   <si>
     <t>MOV R, [R]</t>
   </si>
   <si>
-    <t>MOV a8, [R]</t>
-  </si>
-  <si>
-    <t>MOV a8, a8</t>
-  </si>
-  <si>
     <t>ADD R, d8</t>
   </si>
   <si>
@@ -253,6 +235,78 @@
   </si>
   <si>
     <t>HLT</t>
+  </si>
+  <si>
+    <t>MOV a16,  d8</t>
+  </si>
+  <si>
+    <t>MOV [R], a16</t>
+  </si>
+  <si>
+    <t>MOV a16, [R]</t>
+  </si>
+  <si>
+    <t>MOV a16, R</t>
+  </si>
+  <si>
+    <t>MOV R16, d16</t>
+  </si>
+  <si>
+    <t>MOV R16, R16</t>
+  </si>
+  <si>
+    <t>MOV R16, a16</t>
+  </si>
+  <si>
+    <t>MOV a16,  d16</t>
+  </si>
+  <si>
+    <t>MOV R16, [R16]</t>
+  </si>
+  <si>
+    <t>MOV [R16], [R16]</t>
+  </si>
+  <si>
+    <t>MOV a16, [R16]</t>
+  </si>
+  <si>
+    <t>MOV [R16], R16</t>
+  </si>
+  <si>
+    <t>MOV [R16], d16</t>
+  </si>
+  <si>
+    <t>MOV a16, R16</t>
+  </si>
+  <si>
+    <t>MOV R, a16</t>
+  </si>
+  <si>
+    <t>data types</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>1 byte</t>
+  </si>
+  <si>
+    <t>2 bytes</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>MOV b a16, a16</t>
+  </si>
+  <si>
+    <t>MOV w a16, a16</t>
+  </si>
+  <si>
+    <t>MOV  [R16], a16</t>
   </si>
 </sst>
 </file>
@@ -301,7 +355,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,6 +389,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -562,7 +628,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -574,9 +640,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -587,12 +650,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -661,11 +718,31 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -955,16 +1032,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W17"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="17" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="17" width="11.42578125" customWidth="1"/>
     <col min="19" max="19" width="3.85546875" customWidth="1"/>
     <col min="20" max="20" width="25" customWidth="1"/>
     <col min="21" max="21" width="9.140625" customWidth="1"/>
@@ -973,553 +1053,601 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37"/>
-      <c r="B1" s="35">
+      <c r="A1" s="33"/>
+      <c r="B1" s="32">
         <v>0</v>
       </c>
-      <c r="C1" s="35">
+      <c r="C1" s="32">
         <v>1</v>
       </c>
-      <c r="D1" s="35">
+      <c r="D1" s="32">
         <v>2</v>
       </c>
-      <c r="E1" s="35">
+      <c r="E1" s="32">
         <v>3</v>
       </c>
-      <c r="F1" s="35">
+      <c r="F1" s="32">
         <v>4</v>
       </c>
-      <c r="G1" s="35">
+      <c r="G1" s="32">
         <v>5</v>
       </c>
-      <c r="H1" s="35">
+      <c r="H1" s="32">
         <v>6</v>
       </c>
-      <c r="I1" s="35">
+      <c r="I1" s="32">
         <v>7</v>
       </c>
-      <c r="J1" s="35">
+      <c r="J1" s="32">
         <v>8</v>
       </c>
-      <c r="K1" s="35">
+      <c r="K1" s="32">
         <v>9</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="L1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="M1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="N1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="35" t="s">
+      <c r="O1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="35" t="s">
+      <c r="Q1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="T1" s="35"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" s="36"/>
+    </row>
+    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="14"/>
+      <c r="S2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="U2" s="4"/>
+      <c r="V2" s="9"/>
+      <c r="W2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="32">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="20"/>
+      <c r="S3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="11"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="4" t="s">
+      <c r="T3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U3" s="4"/>
+      <c r="V3" s="10"/>
+      <c r="W3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="32">
+        <v>2</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="14"/>
+      <c r="S4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U4" s="4"/>
+      <c r="V4" s="11"/>
+      <c r="W4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="32">
+        <v>3</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="14"/>
+      <c r="S5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U5" s="4"/>
+    </row>
+    <row r="6" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="32">
+        <v>4</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="14"/>
+    </row>
+    <row r="7" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="32">
+        <v>5</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="14"/>
+    </row>
+    <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="32">
+        <v>6</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="14"/>
+    </row>
+    <row r="9" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="32">
+        <v>7</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="14"/>
+    </row>
+    <row r="10" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="32">
+        <v>8</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="14"/>
+    </row>
+    <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="32">
+        <v>9</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="14"/>
+    </row>
+    <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="14"/>
+    </row>
+    <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="W1" s="4"/>
-    </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35">
-        <v>0</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="17"/>
-      <c r="S2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="U2" s="5"/>
-      <c r="V2" s="12"/>
-      <c r="W2" t="s">
+      <c r="C13" s="27" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="35">
-        <v>1</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="23"/>
-      <c r="S3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U3" s="5"/>
-      <c r="V3" s="13"/>
-      <c r="W3" t="s">
+      <c r="D13" s="28" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35">
+      <c r="E13" s="13"/>
+      <c r="F13" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="14"/>
+    </row>
+    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="17"/>
-      <c r="S4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="U4" s="5"/>
-      <c r="V4" s="14"/>
-      <c r="W4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="35">
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="14"/>
+    </row>
+    <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="26" t="s">
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="14"/>
+    </row>
+    <row r="16" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="17"/>
-      <c r="S5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="U5" s="5"/>
-    </row>
-    <row r="6" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35">
-        <v>4</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="H6" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="17"/>
-    </row>
-    <row r="7" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="35">
-        <v>5</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="17"/>
-    </row>
-    <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="35">
-        <v>6</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="17"/>
-    </row>
-    <row r="9" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="35">
-        <v>7</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="17"/>
-    </row>
-    <row r="10" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="35">
-        <v>8</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="17"/>
-    </row>
-    <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="35">
-        <v>9</v>
-      </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="17"/>
-    </row>
-    <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="17"/>
-    </row>
-    <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="17"/>
-    </row>
-    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="17"/>
-    </row>
-    <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="17"/>
-    </row>
-    <row r="16" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="17" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="33"/>
-      <c r="O17" s="33"/>
-      <c r="P17" s="33"/>
-      <c r="Q17" s="34" t="s">
-        <v>74</v>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B21" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B23" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new instruction set && architecure redesigned 40%
</commit_message>
<xml_diff>
--- a/instruction set.xlsx
+++ b/instruction set.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\desktop\c++\Simple 8-bit CPU emulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E12A0D-3E65-4721-A129-09B373DDF0FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992C441B-AD0D-4836-9DBB-0B07CAE5DF58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="0" windowWidth="22500" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19635" yWindow="1515" windowWidth="18945" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="158">
   <si>
     <t>A</t>
   </si>
@@ -196,6 +196,309 @@
   </si>
   <si>
     <t>16-битный адрес в регистре</t>
+  </si>
+  <si>
+    <t>ADD R, d8</t>
+  </si>
+  <si>
+    <t>ADD R, R</t>
+  </si>
+  <si>
+    <t>ADD R, a16</t>
+  </si>
+  <si>
+    <t>ADD R, [R]</t>
+  </si>
+  <si>
+    <t>ADD R16, d16</t>
+  </si>
+  <si>
+    <t>ADD R16, R16</t>
+  </si>
+  <si>
+    <t>ADD R16, a16</t>
+  </si>
+  <si>
+    <t>ADD R16, [R16]</t>
+  </si>
+  <si>
+    <t>ADD [R], d8</t>
+  </si>
+  <si>
+    <t>ADD [R], R</t>
+  </si>
+  <si>
+    <t>ADD [R], a16</t>
+  </si>
+  <si>
+    <t>ADD [R], [R]</t>
+  </si>
+  <si>
+    <t>ADD [R16], d16</t>
+  </si>
+  <si>
+    <t>ADD [R16], R16</t>
+  </si>
+  <si>
+    <t>ADD  [R16], a16</t>
+  </si>
+  <si>
+    <t>ADD [R16], [R16]</t>
+  </si>
+  <si>
+    <t>ADD a16,  d8</t>
+  </si>
+  <si>
+    <t>ADD a16, R</t>
+  </si>
+  <si>
+    <t>ADD b a16, a16</t>
+  </si>
+  <si>
+    <t>ADD a16, [R]</t>
+  </si>
+  <si>
+    <t>ADD a16,  d16</t>
+  </si>
+  <si>
+    <t>ADD a16, R16</t>
+  </si>
+  <si>
+    <t>ADD w a16, a16</t>
+  </si>
+  <si>
+    <t>ADD a16, [R16]</t>
+  </si>
+  <si>
+    <t>SUB R, d8</t>
+  </si>
+  <si>
+    <t>SUB R, R</t>
+  </si>
+  <si>
+    <t>SUB R, a16</t>
+  </si>
+  <si>
+    <t>SUB R, [R]</t>
+  </si>
+  <si>
+    <t>SUB R16, d16</t>
+  </si>
+  <si>
+    <t>SUB R16, R16</t>
+  </si>
+  <si>
+    <t>SUB R16, a16</t>
+  </si>
+  <si>
+    <t>SUB R16, [R16]</t>
+  </si>
+  <si>
+    <t>SUB [R], d8</t>
+  </si>
+  <si>
+    <t>SUB [R], R</t>
+  </si>
+  <si>
+    <t>SUB [R], a16</t>
+  </si>
+  <si>
+    <t>SUB [R], [R]</t>
+  </si>
+  <si>
+    <t>SUB [R16], d16</t>
+  </si>
+  <si>
+    <t>SUB [R16], R16</t>
+  </si>
+  <si>
+    <t>SUB  [R16], a16</t>
+  </si>
+  <si>
+    <t>SUB [R16], [R16]</t>
+  </si>
+  <si>
+    <t>SUB a16,  d8</t>
+  </si>
+  <si>
+    <t>SUB a16, R</t>
+  </si>
+  <si>
+    <t>SUB b a16, a16</t>
+  </si>
+  <si>
+    <t>SUB a16, [R]</t>
+  </si>
+  <si>
+    <t>SUB a16,  d16</t>
+  </si>
+  <si>
+    <t>SUB a16, R16</t>
+  </si>
+  <si>
+    <t>SUB w a16, a16</t>
+  </si>
+  <si>
+    <t>SUB a16, [R16]</t>
+  </si>
+  <si>
+    <t>JMP a16</t>
+  </si>
+  <si>
+    <t>JMP R/R16</t>
+  </si>
+  <si>
+    <t>JMP [d16]</t>
+  </si>
+  <si>
+    <t>JMP [R/R16]</t>
+  </si>
+  <si>
+    <t>Ооперация перехода</t>
+  </si>
+  <si>
+    <t>CMP R, d8</t>
+  </si>
+  <si>
+    <t>CMP R, R</t>
+  </si>
+  <si>
+    <t>CMP R, a16</t>
+  </si>
+  <si>
+    <t>CMP R, [R]</t>
+  </si>
+  <si>
+    <t>CMP R16, d16</t>
+  </si>
+  <si>
+    <t>CMP R16, R16</t>
+  </si>
+  <si>
+    <t>CMP R16, a16</t>
+  </si>
+  <si>
+    <t>CMP R16, [R16]</t>
+  </si>
+  <si>
+    <t>CMP [R], d8</t>
+  </si>
+  <si>
+    <t>CMP [R], R</t>
+  </si>
+  <si>
+    <t>CMP [R], a16</t>
+  </si>
+  <si>
+    <t>CMP [R], [R]</t>
+  </si>
+  <si>
+    <t>CMP [R16], d16</t>
+  </si>
+  <si>
+    <t>CMP [R16], R16</t>
+  </si>
+  <si>
+    <t>CMP  [R16], a16</t>
+  </si>
+  <si>
+    <t>CMP [R16], [R16]</t>
+  </si>
+  <si>
+    <t>CMP a16,  d8</t>
+  </si>
+  <si>
+    <t>CMP a16, R</t>
+  </si>
+  <si>
+    <t>CMP b a16, a16</t>
+  </si>
+  <si>
+    <t>CMP a16, [R]</t>
+  </si>
+  <si>
+    <t>CMP a16,  d16</t>
+  </si>
+  <si>
+    <t>CMP a16, R16</t>
+  </si>
+  <si>
+    <t>CMP w a16, a16</t>
+  </si>
+  <si>
+    <t>CMP a16, [R16]</t>
+  </si>
+  <si>
+    <t>JE a16</t>
+  </si>
+  <si>
+    <t>JE R/R16</t>
+  </si>
+  <si>
+    <t>JE [d16]</t>
+  </si>
+  <si>
+    <t>JE [R/R16]</t>
+  </si>
+  <si>
+    <t>JNE a16</t>
+  </si>
+  <si>
+    <t>JNE R/R16</t>
+  </si>
+  <si>
+    <t>JNE [d16]</t>
+  </si>
+  <si>
+    <t>JNE [R/R16]</t>
+  </si>
+  <si>
+    <t>JL a16</t>
+  </si>
+  <si>
+    <t>JL R/R16</t>
+  </si>
+  <si>
+    <t>JL [d16]</t>
+  </si>
+  <si>
+    <t>JL [R/R16]</t>
+  </si>
+  <si>
+    <t>JG a16</t>
+  </si>
+  <si>
+    <t>JG R/R16</t>
+  </si>
+  <si>
+    <t>JG [d16]</t>
+  </si>
+  <si>
+    <t>JG [R/R16]</t>
+  </si>
+  <si>
+    <t>JLE a16</t>
+  </si>
+  <si>
+    <t>JLE R/R16</t>
+  </si>
+  <si>
+    <t>JLE [d16]</t>
+  </si>
+  <si>
+    <t>JLE [R/R16]</t>
+  </si>
+  <si>
+    <t>JGE a16</t>
+  </si>
+  <si>
+    <t>JGE R/R16</t>
+  </si>
+  <si>
+    <t>JGE [d16]</t>
+  </si>
+  <si>
+    <t>JGE [R/R16]</t>
   </si>
 </sst>
 </file>
@@ -244,7 +547,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,8 +587,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -528,6 +837,346 @@
         <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -537,7 +1186,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -555,24 +1204,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -580,15 +1217,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -597,23 +1225,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
@@ -639,6 +1255,169 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="29" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="36" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Нейтральный" xfId="3" builtinId="28"/>
@@ -929,8 +1708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,7 +1718,17 @@
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="17" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" customWidth="1"/>
     <col min="18" max="18" width="8.7109375" customWidth="1"/>
     <col min="19" max="19" width="6.28515625" customWidth="1"/>
     <col min="20" max="20" width="28.28515625" customWidth="1"/>
@@ -949,87 +1738,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20"/>
-      <c r="B1" s="19">
+      <c r="A1" s="13"/>
+      <c r="B1" s="12">
         <v>0</v>
       </c>
-      <c r="C1" s="19">
+      <c r="C1" s="12">
         <v>1</v>
       </c>
-      <c r="D1" s="19">
+      <c r="D1" s="12">
         <v>2</v>
       </c>
-      <c r="E1" s="19">
+      <c r="E1" s="12">
         <v>3</v>
       </c>
-      <c r="F1" s="19">
+      <c r="F1" s="12">
         <v>4</v>
       </c>
-      <c r="G1" s="19">
+      <c r="G1" s="12">
         <v>5</v>
       </c>
-      <c r="H1" s="19">
+      <c r="H1" s="12">
         <v>6</v>
       </c>
-      <c r="I1" s="19">
+      <c r="I1" s="12">
         <v>7</v>
       </c>
-      <c r="J1" s="19">
+      <c r="J1" s="12">
         <v>8</v>
       </c>
-      <c r="K1" s="19">
+      <c r="K1" s="12">
         <v>9</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="M1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="N1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="O1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="P1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="Q1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="25" t="s">
+      <c r="S1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="26"/>
+      <c r="T1" s="29"/>
       <c r="U1" s="4"/>
-      <c r="V1" s="25" t="s">
+      <c r="V1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="26"/>
+      <c r="W1" s="29"/>
     </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19">
+    <row r="2" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2" s="88"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="9"/>
       <c r="S2" s="6" t="s">
         <v>12</v>
       </c>
@@ -1037,37 +1844,49 @@
         <v>13</v>
       </c>
       <c r="U2" s="3"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="32" t="s">
+      <c r="V2" s="20"/>
+      <c r="W2" s="21" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19">
+      <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="13"/>
+      <c r="B3" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="K3" s="85"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="9"/>
       <c r="S3" s="6" t="s">
         <v>49</v>
       </c>
@@ -1075,37 +1894,49 @@
         <v>50</v>
       </c>
       <c r="U3" s="3"/>
-      <c r="V3" s="28"/>
-      <c r="W3" s="27" t="s">
+      <c r="V3" s="17"/>
+      <c r="W3" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19">
+      <c r="A4" s="12">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="9"/>
+      <c r="B4" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="J4" s="52" t="s">
+        <v>99</v>
+      </c>
+      <c r="K4" s="85"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="83"/>
+      <c r="P4" s="84"/>
+      <c r="Q4" s="8"/>
       <c r="S4" s="5" t="s">
         <v>48</v>
       </c>
@@ -1113,37 +1944,49 @@
         <v>51</v>
       </c>
       <c r="U4" s="3"/>
-      <c r="V4" s="29"/>
-      <c r="W4" s="30" t="s">
-        <v>23</v>
+      <c r="V4" s="18"/>
+      <c r="W4" s="19" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19">
+      <c r="A5" s="12">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="9"/>
+      <c r="B5" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="J5" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="K5" s="85"/>
+      <c r="L5" s="82"/>
+      <c r="M5" s="83"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="83"/>
+      <c r="P5" s="84"/>
+      <c r="Q5" s="8"/>
       <c r="S5" s="5" t="s">
         <v>48</v>
       </c>
@@ -1151,33 +1994,49 @@
         <v>52</v>
       </c>
       <c r="U5" s="3"/>
+      <c r="V5" s="61"/>
+      <c r="W5" s="62" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19">
+      <c r="A6" s="12">
         <v>4</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="9"/>
+      <c r="B6" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="J6" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="K6" s="85"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="83"/>
+      <c r="N6" s="83"/>
+      <c r="O6" s="83"/>
+      <c r="P6" s="84"/>
+      <c r="Q6" s="8"/>
       <c r="S6" s="5" t="s">
         <v>14</v>
       </c>
@@ -1186,31 +2045,43 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="19">
+      <c r="A7" s="12">
         <v>5</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="9"/>
+      <c r="B7" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="J7" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="K7" s="85"/>
+      <c r="L7" s="82"/>
+      <c r="M7" s="83"/>
+      <c r="N7" s="83"/>
+      <c r="O7" s="83"/>
+      <c r="P7" s="84"/>
+      <c r="Q7" s="8"/>
       <c r="S7" s="5" t="s">
         <v>53</v>
       </c>
@@ -1219,259 +2090,381 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19">
+      <c r="A8" s="12">
         <v>6</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="9"/>
-      <c r="S8" s="33" t="s">
+      <c r="B8" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="I8" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="J8" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="K8" s="85"/>
+      <c r="L8" s="82"/>
+      <c r="M8" s="83"/>
+      <c r="N8" s="83"/>
+      <c r="O8" s="83"/>
+      <c r="P8" s="84"/>
+      <c r="Q8" s="8"/>
+      <c r="S8" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="T8" s="34" t="s">
+      <c r="T8" s="23" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19">
+      <c r="A9" s="12">
         <v>7</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="9"/>
-      <c r="S9" s="33" t="s">
+      <c r="B9" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="I9" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="J9" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" s="85"/>
+      <c r="L9" s="82"/>
+      <c r="M9" s="83"/>
+      <c r="N9" s="83"/>
+      <c r="O9" s="83"/>
+      <c r="P9" s="84"/>
+      <c r="Q9" s="8"/>
+      <c r="S9" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="T9" s="34" t="s">
+      <c r="T9" s="23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="19">
+    <row r="10" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12">
         <v>8</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="9"/>
-      <c r="S10" s="35" t="s">
+      <c r="B10" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" s="64" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10" s="30"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="83"/>
+      <c r="L10" s="83"/>
+      <c r="M10" s="83"/>
+      <c r="N10" s="83"/>
+      <c r="O10" s="83"/>
+      <c r="P10" s="84"/>
+      <c r="Q10" s="8"/>
+      <c r="S10" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="T10" s="36" t="s">
+      <c r="T10" s="25" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="19">
+      <c r="A11" s="12">
         <v>9</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="9"/>
-      <c r="S11" s="37" t="s">
+      <c r="B11" s="66" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="67" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="68" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="31"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="83"/>
+      <c r="O11" s="83"/>
+      <c r="P11" s="84"/>
+      <c r="Q11" s="8"/>
+      <c r="S11" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="T11" s="38" t="s">
+      <c r="T11" s="27" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="9"/>
+      <c r="B12" s="66" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="70" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="31"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="83"/>
+      <c r="O12" s="83"/>
+      <c r="P12" s="84"/>
+      <c r="Q12" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="9"/>
+      <c r="B13" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="67" t="s">
+        <v>121</v>
+      </c>
+      <c r="D13" s="70" t="s">
+        <v>129</v>
+      </c>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="83"/>
+      <c r="O13" s="83"/>
+      <c r="P13" s="84"/>
+      <c r="Q13" s="86" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="s">
+    <row r="14" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="9"/>
+      <c r="B14" s="66" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" s="69" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" s="72" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" s="31"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="58" t="s">
+        <v>105</v>
+      </c>
+      <c r="L14" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="M14" s="58" t="s">
+        <v>138</v>
+      </c>
+      <c r="N14" s="58" t="s">
+        <v>142</v>
+      </c>
+      <c r="O14" s="58" t="s">
+        <v>146</v>
+      </c>
+      <c r="P14" s="58" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q14" s="58" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="9"/>
+      <c r="B15" s="66" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="67" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="L15" s="59" t="s">
+        <v>135</v>
+      </c>
+      <c r="M15" s="59" t="s">
+        <v>139</v>
+      </c>
+      <c r="N15" s="59" t="s">
+        <v>143</v>
+      </c>
+      <c r="O15" s="59" t="s">
+        <v>147</v>
+      </c>
+      <c r="P15" s="59" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q15" s="59" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="16" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="9" t="s">
-        <v>25</v>
+      <c r="B16" s="66" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="69" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" s="70" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="L16" s="59" t="s">
+        <v>136</v>
+      </c>
+      <c r="M16" s="59" t="s">
+        <v>140</v>
+      </c>
+      <c r="N16" s="59" t="s">
+        <v>144</v>
+      </c>
+      <c r="O16" s="59" t="s">
+        <v>148</v>
+      </c>
+      <c r="P16" s="59" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q16" s="59" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="18" t="s">
-        <v>24</v>
+      <c r="B17" s="73" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="74" t="s">
+        <v>125</v>
+      </c>
+      <c r="D17" s="75" t="s">
+        <v>133</v>
+      </c>
+      <c r="E17" s="76"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="78"/>
+      <c r="I17" s="78"/>
+      <c r="J17" s="78"/>
+      <c r="K17" s="60" t="s">
+        <v>108</v>
+      </c>
+      <c r="L17" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="M17" s="60" t="s">
+        <v>141</v>
+      </c>
+      <c r="N17" s="60" t="s">
+        <v>145</v>
+      </c>
+      <c r="O17" s="60" t="s">
+        <v>149</v>
+      </c>
+      <c r="P17" s="60" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q17" s="60" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement memory rights, stack, new instructions
</commit_message>
<xml_diff>
--- a/instruction set.xlsx
+++ b/instruction set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\desktop\c++\Simple 8-bit CPU emulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992C441B-AD0D-4836-9DBB-0B07CAE5DF58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25712FBC-89CA-4485-8990-8DE920210634}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19635" yWindow="1515" windowWidth="18945" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="171">
   <si>
     <t>A</t>
   </si>
@@ -499,6 +499,45 @@
   </si>
   <si>
     <t>JGE [R/R16]</t>
+  </si>
+  <si>
+    <t>PUSH d8</t>
+  </si>
+  <si>
+    <t>PUSH R</t>
+  </si>
+  <si>
+    <t>PUSH [R]</t>
+  </si>
+  <si>
+    <t>PUSH d16</t>
+  </si>
+  <si>
+    <t>PUSH R16</t>
+  </si>
+  <si>
+    <t>PUSH [R16]</t>
+  </si>
+  <si>
+    <t>POP R</t>
+  </si>
+  <si>
+    <t>POP [R]</t>
+  </si>
+  <si>
+    <t>POP R16</t>
+  </si>
+  <si>
+    <t>POP [R16]</t>
+  </si>
+  <si>
+    <t>PUSH [a16]</t>
+  </si>
+  <si>
+    <t>POP b [a16]</t>
+  </si>
+  <si>
+    <t>POP w [a16]</t>
   </si>
 </sst>
 </file>
@@ -1186,7 +1225,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1255,12 +1294,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1410,14 +1443,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Нейтральный" xfId="3" builtinId="28"/>
@@ -1708,8 +1745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1787,54 +1824,56 @@
       <c r="Q1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="28" t="s">
+      <c r="S1" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="29"/>
+      <c r="T1" s="86"/>
       <c r="U1" s="4"/>
-      <c r="V1" s="28" t="s">
+      <c r="V1" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="29"/>
+      <c r="W1" s="86"/>
     </row>
     <row r="2" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>0</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="47" t="s">
+      <c r="E2" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="47" t="s">
+      <c r="H2" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="I2" s="48" t="s">
+      <c r="I2" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="J2" s="49" t="s">
+      <c r="J2" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="K2" s="88"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="87" t="s">
+      <c r="K2" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="L2" s="77"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="79"/>
+      <c r="Q2" s="84" t="s">
         <v>6</v>
       </c>
       <c r="S2" s="6" t="s">
@@ -1853,39 +1892,43 @@
       <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="37" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="51" t="s">
+      <c r="G3" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="50" t="s">
+      <c r="H3" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="J3" s="51" t="s">
+      <c r="J3" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="K3" s="85"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="83"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="84"/>
+      <c r="K3" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="L3" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="82"/>
       <c r="Q3" s="9"/>
       <c r="S3" s="6" t="s">
         <v>49</v>
@@ -1903,39 +1946,43 @@
       <c r="A4" s="12">
         <v>2</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="37" t="s">
         <v>40</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="52" t="s">
+      <c r="G4" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="I4" s="34" t="s">
+      <c r="I4" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="J4" s="52" t="s">
+      <c r="J4" s="50" t="s">
         <v>99</v>
       </c>
-      <c r="K4" s="85"/>
-      <c r="L4" s="82"/>
-      <c r="M4" s="83"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="83"/>
-      <c r="P4" s="84"/>
+      <c r="K4" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="L4" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="82"/>
       <c r="Q4" s="8"/>
       <c r="S4" s="5" t="s">
         <v>48</v>
@@ -1953,39 +2000,43 @@
       <c r="A5" s="12">
         <v>3</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="40" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="G5" s="52" t="s">
+      <c r="G5" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="J5" s="52" t="s">
+      <c r="J5" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="K5" s="85"/>
-      <c r="L5" s="82"/>
-      <c r="M5" s="83"/>
-      <c r="N5" s="83"/>
-      <c r="O5" s="83"/>
-      <c r="P5" s="84"/>
+      <c r="K5" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="L5" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="82"/>
       <c r="Q5" s="8"/>
       <c r="S5" s="5" t="s">
         <v>48</v>
@@ -1994,8 +2045,8 @@
         <v>52</v>
       </c>
       <c r="U5" s="3"/>
-      <c r="V5" s="61"/>
-      <c r="W5" s="62" t="s">
+      <c r="V5" s="59"/>
+      <c r="W5" s="60" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2003,39 +2054,41 @@
       <c r="A6" s="12">
         <v>4</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="37" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="D6" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="50" t="s">
+      <c r="E6" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="G6" s="54" t="s">
+      <c r="G6" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="H6" s="50" t="s">
+      <c r="H6" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="I6" s="34" t="s">
+      <c r="I6" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="J6" s="54" t="s">
+      <c r="J6" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="K6" s="85"/>
-      <c r="L6" s="82"/>
-      <c r="M6" s="83"/>
-      <c r="N6" s="83"/>
-      <c r="O6" s="83"/>
-      <c r="P6" s="84"/>
+      <c r="K6" s="37" t="s">
+        <v>161</v>
+      </c>
+      <c r="L6" s="80"/>
+      <c r="M6" s="81"/>
+      <c r="N6" s="81"/>
+      <c r="O6" s="81"/>
+      <c r="P6" s="82"/>
       <c r="Q6" s="8"/>
       <c r="S6" s="5" t="s">
         <v>14</v>
@@ -2048,39 +2101,43 @@
       <c r="A7" s="12">
         <v>5</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="37" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="50" t="s">
+      <c r="E7" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="51" t="s">
+      <c r="G7" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="H7" s="50" t="s">
+      <c r="H7" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="35" t="s">
+      <c r="I7" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="J7" s="51" t="s">
+      <c r="J7" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="K7" s="85"/>
-      <c r="L7" s="82"/>
-      <c r="M7" s="83"/>
-      <c r="N7" s="83"/>
-      <c r="O7" s="83"/>
-      <c r="P7" s="84"/>
+      <c r="K7" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="L7" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="M7" s="81"/>
+      <c r="N7" s="81"/>
+      <c r="O7" s="81"/>
+      <c r="P7" s="82"/>
       <c r="Q7" s="8"/>
       <c r="S7" s="5" t="s">
         <v>53</v>
@@ -2093,39 +2150,43 @@
       <c r="A8" s="12">
         <v>6</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="37" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="50" t="s">
+      <c r="E8" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="G8" s="52" t="s">
+      <c r="G8" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="H8" s="50" t="s">
+      <c r="H8" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="J8" s="52" t="s">
+      <c r="J8" s="50" t="s">
         <v>103</v>
       </c>
-      <c r="K8" s="85"/>
-      <c r="L8" s="82"/>
-      <c r="M8" s="83"/>
-      <c r="N8" s="83"/>
-      <c r="O8" s="83"/>
-      <c r="P8" s="84"/>
+      <c r="K8" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="L8" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="M8" s="81"/>
+      <c r="N8" s="81"/>
+      <c r="O8" s="81"/>
+      <c r="P8" s="82"/>
       <c r="Q8" s="8"/>
       <c r="S8" s="22" t="s">
         <v>16</v>
@@ -2138,39 +2199,43 @@
       <c r="A9" s="12">
         <v>7</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="55" t="s">
+      <c r="E9" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="56" t="s">
+      <c r="F9" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="G9" s="57" t="s">
+      <c r="G9" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="H9" s="55" t="s">
+      <c r="H9" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="I9" s="56" t="s">
+      <c r="I9" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="J9" s="57" t="s">
+      <c r="J9" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="K9" s="85"/>
-      <c r="L9" s="82"/>
-      <c r="M9" s="83"/>
-      <c r="N9" s="83"/>
-      <c r="O9" s="83"/>
-      <c r="P9" s="84"/>
+      <c r="K9" s="42" t="s">
+        <v>163</v>
+      </c>
+      <c r="L9" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="M9" s="81"/>
+      <c r="N9" s="81"/>
+      <c r="O9" s="81"/>
+      <c r="P9" s="82"/>
       <c r="Q9" s="8"/>
       <c r="S9" s="22" t="s">
         <v>55</v>
@@ -2183,27 +2248,27 @@
       <c r="A10" s="12">
         <v>8</v>
       </c>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="C10" s="62" t="s">
         <v>118</v>
       </c>
-      <c r="D10" s="65" t="s">
+      <c r="D10" s="63" t="s">
         <v>126</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="83"/>
-      <c r="L10" s="83"/>
-      <c r="M10" s="83"/>
-      <c r="N10" s="83"/>
-      <c r="O10" s="83"/>
-      <c r="P10" s="84"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="81"/>
+      <c r="L10" s="81"/>
+      <c r="M10" s="81"/>
+      <c r="N10" s="81"/>
+      <c r="O10" s="81"/>
+      <c r="P10" s="82"/>
       <c r="Q10" s="8"/>
       <c r="S10" s="24" t="s">
         <v>47</v>
@@ -2216,27 +2281,27 @@
       <c r="A11" s="12">
         <v>9</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="64" t="s">
         <v>111</v>
       </c>
-      <c r="C11" s="67" t="s">
+      <c r="C11" s="65" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="68" t="s">
+      <c r="D11" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
       <c r="K11" s="14"/>
       <c r="L11" s="15"/>
       <c r="M11" s="15"/>
-      <c r="N11" s="83"/>
-      <c r="O11" s="83"/>
-      <c r="P11" s="84"/>
+      <c r="N11" s="81"/>
+      <c r="O11" s="81"/>
+      <c r="P11" s="82"/>
       <c r="Q11" s="8"/>
       <c r="S11" s="26" t="s">
         <v>41</v>
@@ -2249,27 +2314,27 @@
       <c r="A12" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="69" t="s">
+      <c r="C12" s="67" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="68" t="s">
         <v>128</v>
       </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
-      <c r="N12" s="83"/>
-      <c r="O12" s="83"/>
-      <c r="P12" s="84"/>
+      <c r="N12" s="81"/>
+      <c r="O12" s="81"/>
+      <c r="P12" s="82"/>
       <c r="Q12" s="8" t="s">
         <v>25</v>
       </c>
@@ -2278,28 +2343,28 @@
       <c r="A13" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="69" t="s">
         <v>113</v>
       </c>
-      <c r="C13" s="67" t="s">
+      <c r="C13" s="65" t="s">
         <v>121</v>
       </c>
-      <c r="D13" s="70" t="s">
+      <c r="D13" s="68" t="s">
         <v>129</v>
       </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
-      <c r="N13" s="83"/>
-      <c r="O13" s="83"/>
-      <c r="P13" s="84"/>
-      <c r="Q13" s="86" t="s">
+      <c r="N13" s="81"/>
+      <c r="O13" s="81"/>
+      <c r="P13" s="82"/>
+      <c r="Q13" s="83" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2307,40 +2372,40 @@
       <c r="A14" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="69" t="s">
+      <c r="C14" s="67" t="s">
         <v>122</v>
       </c>
-      <c r="D14" s="72" t="s">
+      <c r="D14" s="70" t="s">
         <v>130</v>
       </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="58" t="s">
+      <c r="E14" s="29"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="L14" s="58" t="s">
+      <c r="L14" s="56" t="s">
         <v>134</v>
       </c>
-      <c r="M14" s="58" t="s">
+      <c r="M14" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="N14" s="58" t="s">
+      <c r="N14" s="56" t="s">
         <v>142</v>
       </c>
-      <c r="O14" s="58" t="s">
+      <c r="O14" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="P14" s="58" t="s">
+      <c r="P14" s="56" t="s">
         <v>150</v>
       </c>
-      <c r="Q14" s="58" t="s">
+      <c r="Q14" s="56" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2348,40 +2413,40 @@
       <c r="A15" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="D15" s="68" t="s">
+      <c r="D15" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="59" t="s">
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="L15" s="59" t="s">
+      <c r="L15" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="M15" s="59" t="s">
+      <c r="M15" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="N15" s="59" t="s">
+      <c r="N15" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="O15" s="59" t="s">
+      <c r="O15" s="57" t="s">
         <v>147</v>
       </c>
-      <c r="P15" s="59" t="s">
+      <c r="P15" s="57" t="s">
         <v>151</v>
       </c>
-      <c r="Q15" s="59" t="s">
+      <c r="Q15" s="57" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2389,40 +2454,40 @@
       <c r="A16" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="C16" s="69" t="s">
+      <c r="C16" s="67" t="s">
         <v>124</v>
       </c>
-      <c r="D16" s="70" t="s">
+      <c r="D16" s="68" t="s">
         <v>132</v>
       </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="59" t="s">
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="L16" s="59" t="s">
+      <c r="L16" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="M16" s="59" t="s">
+      <c r="M16" s="57" t="s">
         <v>140</v>
       </c>
-      <c r="N16" s="59" t="s">
+      <c r="N16" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="O16" s="59" t="s">
+      <c r="O16" s="57" t="s">
         <v>148</v>
       </c>
-      <c r="P16" s="59" t="s">
+      <c r="P16" s="57" t="s">
         <v>152</v>
       </c>
-      <c r="Q16" s="59" t="s">
+      <c r="Q16" s="57" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2430,40 +2495,40 @@
       <c r="A17" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="C17" s="74" t="s">
+      <c r="C17" s="72" t="s">
         <v>125</v>
       </c>
-      <c r="D17" s="75" t="s">
+      <c r="D17" s="73" t="s">
         <v>133</v>
       </c>
-      <c r="E17" s="76"/>
-      <c r="F17" s="77"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="78"/>
-      <c r="J17" s="78"/>
-      <c r="K17" s="60" t="s">
+      <c r="E17" s="74"/>
+      <c r="F17" s="75"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="76"/>
+      <c r="I17" s="76"/>
+      <c r="J17" s="76"/>
+      <c r="K17" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="L17" s="60" t="s">
+      <c r="L17" s="58" t="s">
         <v>137</v>
       </c>
-      <c r="M17" s="60" t="s">
+      <c r="M17" s="58" t="s">
         <v>141</v>
       </c>
-      <c r="N17" s="60" t="s">
+      <c r="N17" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="O17" s="60" t="s">
+      <c r="O17" s="58" t="s">
         <v>149</v>
       </c>
-      <c r="P17" s="60" t="s">
+      <c r="P17" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="Q17" s="60" t="s">
+      <c r="Q17" s="58" t="s">
         <v>157</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new instructions & new parser & memory rights
</commit_message>
<xml_diff>
--- a/instruction set.xlsx
+++ b/instruction set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\desktop\c++\Simple 8-bit CPU emulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25712FBC-89CA-4485-8990-8DE920210634}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DCFAFC-00E2-4D59-81B0-C65ED484A951}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1746,7 +1746,7 @@
   <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
stack protection , call, ret
</commit_message>
<xml_diff>
--- a/instruction set.xlsx
+++ b/instruction set.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\desktop\c++\Simple 8-bit CPU emulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DCFAFC-00E2-4D59-81B0-C65ED484A951}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3299EDC1-B61F-4258-98E3-F417C0136A7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="176">
   <si>
     <t>A</t>
   </si>
@@ -538,6 +538,21 @@
   </si>
   <si>
     <t>POP w [a16]</t>
+  </si>
+  <si>
+    <t>CALL a16</t>
+  </si>
+  <si>
+    <t>CALL R/R16</t>
+  </si>
+  <si>
+    <t>CALL [d16]</t>
+  </si>
+  <si>
+    <t>CALL [R/R16]</t>
+  </si>
+  <si>
+    <t>RET</t>
   </si>
 </sst>
 </file>
@@ -1225,7 +1240,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1263,9 +1278,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1746,7 +1758,7 @@
   <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1761,7 +1773,8 @@
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="13" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="12" max="13" width="11.42578125" customWidth="1"/>
     <col min="14" max="14" width="14.140625" customWidth="1"/>
     <col min="15" max="15" width="14.7109375" customWidth="1"/>
     <col min="16" max="16" width="15.140625" customWidth="1"/>
@@ -1824,56 +1837,56 @@
       <c r="Q1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="85" t="s">
+      <c r="S1" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="86"/>
+      <c r="T1" s="85"/>
       <c r="U1" s="4"/>
-      <c r="V1" s="85" t="s">
+      <c r="V1" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="86"/>
+      <c r="W1" s="85"/>
     </row>
     <row r="2" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>0</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="45" t="s">
+      <c r="H2" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="I2" s="46" t="s">
+      <c r="I2" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="J2" s="47" t="s">
+      <c r="J2" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="K2" s="34" t="s">
+      <c r="K2" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="L2" s="77"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="84" t="s">
+      <c r="L2" s="76"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="83" t="s">
         <v>6</v>
       </c>
       <c r="S2" s="6" t="s">
@@ -1883,8 +1896,8 @@
         <v>13</v>
       </c>
       <c r="U2" s="3"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="21" t="s">
+      <c r="V2" s="19"/>
+      <c r="W2" s="20" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1892,43 +1905,43 @@
       <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="H3" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="J3" s="49" t="s">
+      <c r="J3" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="K3" s="37" t="s">
+      <c r="K3" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="L3" s="37" t="s">
+      <c r="L3" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
-      <c r="P3" s="82"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="80"/>
+      <c r="O3" s="80"/>
+      <c r="P3" s="81"/>
       <c r="Q3" s="9"/>
       <c r="S3" s="6" t="s">
         <v>49</v>
@@ -1937,8 +1950,8 @@
         <v>50</v>
       </c>
       <c r="U3" s="3"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="16" t="s">
+      <c r="V3" s="16"/>
+      <c r="W3" s="15" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1946,43 +1959,43 @@
       <c r="A4" s="12">
         <v>2</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>40</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="50" t="s">
+      <c r="G4" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="H4" s="48" t="s">
+      <c r="H4" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="J4" s="50" t="s">
+      <c r="J4" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="K4" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="L4" s="37" t="s">
+      <c r="L4" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="82"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="81"/>
       <c r="Q4" s="8"/>
       <c r="S4" s="5" t="s">
         <v>48</v>
@@ -1991,8 +2004,8 @@
         <v>51</v>
       </c>
       <c r="U4" s="3"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="19" t="s">
+      <c r="V4" s="17"/>
+      <c r="W4" s="18" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2000,43 +2013,43 @@
       <c r="A5" s="12">
         <v>3</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="39" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="33" t="s">
+      <c r="F5" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="G5" s="50" t="s">
+      <c r="G5" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="51" t="s">
+      <c r="H5" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="I5" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="J5" s="50" t="s">
+      <c r="J5" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="K5" s="40" t="s">
+      <c r="K5" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="L5" s="40" t="s">
+      <c r="L5" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="82"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="80"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="81"/>
       <c r="Q5" s="8"/>
       <c r="S5" s="5" t="s">
         <v>48</v>
@@ -2045,8 +2058,8 @@
         <v>52</v>
       </c>
       <c r="U5" s="3"/>
-      <c r="V5" s="59"/>
-      <c r="W5" s="60" t="s">
+      <c r="V5" s="58"/>
+      <c r="W5" s="59" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2054,41 +2067,41 @@
       <c r="A6" s="12">
         <v>4</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="36" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="E6" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="G6" s="52" t="s">
+      <c r="G6" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="H6" s="48" t="s">
+      <c r="H6" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="I6" s="32" t="s">
+      <c r="I6" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="J6" s="52" t="s">
+      <c r="J6" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="K6" s="37" t="s">
+      <c r="K6" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="L6" s="80"/>
-      <c r="M6" s="81"/>
-      <c r="N6" s="81"/>
-      <c r="O6" s="81"/>
-      <c r="P6" s="82"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="80"/>
+      <c r="N6" s="80"/>
+      <c r="O6" s="80"/>
+      <c r="P6" s="81"/>
       <c r="Q6" s="8"/>
       <c r="S6" s="5" t="s">
         <v>14</v>
@@ -2101,43 +2114,43 @@
       <c r="A7" s="12">
         <v>5</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="36" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="49" t="s">
+      <c r="G7" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="H7" s="48" t="s">
+      <c r="H7" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="I7" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="J7" s="49" t="s">
+      <c r="J7" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="K7" s="37" t="s">
+      <c r="K7" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="L7" s="37" t="s">
+      <c r="L7" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="M7" s="81"/>
-      <c r="N7" s="81"/>
-      <c r="O7" s="81"/>
-      <c r="P7" s="82"/>
+      <c r="M7" s="80"/>
+      <c r="N7" s="80"/>
+      <c r="O7" s="80"/>
+      <c r="P7" s="81"/>
       <c r="Q7" s="8"/>
       <c r="S7" s="5" t="s">
         <v>53</v>
@@ -2150,48 +2163,48 @@
       <c r="A8" s="12">
         <v>6</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="36" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="48" t="s">
+      <c r="E8" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="G8" s="50" t="s">
+      <c r="G8" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="H8" s="48" t="s">
+      <c r="H8" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="J8" s="50" t="s">
+      <c r="J8" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="K8" s="37" t="s">
+      <c r="K8" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="L8" s="37" t="s">
+      <c r="L8" s="36" t="s">
         <v>170</v>
       </c>
-      <c r="M8" s="81"/>
-      <c r="N8" s="81"/>
-      <c r="O8" s="81"/>
-      <c r="P8" s="82"/>
+      <c r="M8" s="80"/>
+      <c r="N8" s="80"/>
+      <c r="O8" s="80"/>
+      <c r="P8" s="81"/>
       <c r="Q8" s="8"/>
-      <c r="S8" s="22" t="s">
+      <c r="S8" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="T8" s="23" t="s">
+      <c r="T8" s="22" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2199,48 +2212,48 @@
       <c r="A9" s="12">
         <v>7</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="53" t="s">
+      <c r="E9" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="54" t="s">
+      <c r="F9" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="G9" s="55" t="s">
+      <c r="G9" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="H9" s="53" t="s">
+      <c r="H9" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="I9" s="54" t="s">
+      <c r="I9" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="J9" s="55" t="s">
+      <c r="J9" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="K9" s="42" t="s">
+      <c r="K9" s="41" t="s">
         <v>163</v>
       </c>
-      <c r="L9" s="42" t="s">
+      <c r="L9" s="41" t="s">
         <v>167</v>
       </c>
-      <c r="M9" s="81"/>
-      <c r="N9" s="81"/>
-      <c r="O9" s="81"/>
-      <c r="P9" s="82"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="80"/>
+      <c r="O9" s="80"/>
+      <c r="P9" s="81"/>
       <c r="Q9" s="8"/>
-      <c r="S9" s="22" t="s">
+      <c r="S9" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="T9" s="23" t="s">
+      <c r="T9" s="22" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2248,65 +2261,71 @@
       <c r="A10" s="12">
         <v>8</v>
       </c>
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="62" t="s">
+      <c r="C10" s="61" t="s">
         <v>118</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="62" t="s">
         <v>126</v>
       </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="81"/>
-      <c r="L10" s="81"/>
-      <c r="M10" s="81"/>
-      <c r="N10" s="81"/>
-      <c r="O10" s="81"/>
-      <c r="P10" s="82"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="L10" s="80"/>
+      <c r="M10" s="80"/>
+      <c r="N10" s="80"/>
+      <c r="O10" s="80"/>
+      <c r="P10" s="81"/>
       <c r="Q10" s="8"/>
-      <c r="S10" s="24" t="s">
+      <c r="S10" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="T10" s="25" t="s">
+      <c r="T10" s="24" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>9</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="64" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="66" t="s">
+      <c r="D11" s="65" t="s">
         <v>127</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="81"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="82"/>
-      <c r="Q11" s="8"/>
-      <c r="S11" s="26" t="s">
+      <c r="E11" s="28"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="80"/>
+      <c r="O11" s="80"/>
+      <c r="P11" s="81"/>
+      <c r="Q11" s="55" t="s">
+        <v>175</v>
+      </c>
+      <c r="S11" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="T11" s="27" t="s">
+      <c r="T11" s="26" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2314,27 +2333,29 @@
       <c r="A12" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="67" t="s">
+      <c r="C12" s="66" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="68" t="s">
+      <c r="D12" s="67" t="s">
         <v>128</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="7"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="56" t="s">
+        <v>173</v>
+      </c>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
-      <c r="N12" s="81"/>
-      <c r="O12" s="81"/>
-      <c r="P12" s="82"/>
+      <c r="N12" s="80"/>
+      <c r="O12" s="80"/>
+      <c r="P12" s="81"/>
       <c r="Q12" s="8" t="s">
         <v>25</v>
       </c>
@@ -2343,28 +2364,30 @@
       <c r="A13" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="69" t="s">
+      <c r="B13" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="C13" s="65" t="s">
+      <c r="C13" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="D13" s="68" t="s">
+      <c r="D13" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="7"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="57" t="s">
+        <v>174</v>
+      </c>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
-      <c r="N13" s="81"/>
-      <c r="O13" s="81"/>
-      <c r="P13" s="82"/>
-      <c r="Q13" s="83" t="s">
+      <c r="N13" s="80"/>
+      <c r="O13" s="80"/>
+      <c r="P13" s="81"/>
+      <c r="Q13" s="82" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2372,40 +2395,40 @@
       <c r="A14" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="67" t="s">
+      <c r="C14" s="66" t="s">
         <v>122</v>
       </c>
-      <c r="D14" s="70" t="s">
+      <c r="D14" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="56" t="s">
+      <c r="E14" s="28"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="L14" s="56" t="s">
+      <c r="L14" s="55" t="s">
         <v>134</v>
       </c>
-      <c r="M14" s="56" t="s">
+      <c r="M14" s="55" t="s">
         <v>138</v>
       </c>
-      <c r="N14" s="56" t="s">
+      <c r="N14" s="55" t="s">
         <v>142</v>
       </c>
-      <c r="O14" s="56" t="s">
+      <c r="O14" s="55" t="s">
         <v>146</v>
       </c>
-      <c r="P14" s="56" t="s">
+      <c r="P14" s="55" t="s">
         <v>150</v>
       </c>
-      <c r="Q14" s="56" t="s">
+      <c r="Q14" s="55" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2413,40 +2436,40 @@
       <c r="A15" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="C15" s="65" t="s">
+      <c r="C15" s="64" t="s">
         <v>123</v>
       </c>
-      <c r="D15" s="66" t="s">
+      <c r="D15" s="65" t="s">
         <v>131</v>
       </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="57" t="s">
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="L15" s="57" t="s">
+      <c r="L15" s="56" t="s">
         <v>135</v>
       </c>
-      <c r="M15" s="57" t="s">
+      <c r="M15" s="56" t="s">
         <v>139</v>
       </c>
-      <c r="N15" s="57" t="s">
+      <c r="N15" s="56" t="s">
         <v>143</v>
       </c>
-      <c r="O15" s="57" t="s">
+      <c r="O15" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="P15" s="57" t="s">
+      <c r="P15" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="Q15" s="57" t="s">
+      <c r="Q15" s="56" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2454,40 +2477,40 @@
       <c r="A16" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="63" t="s">
         <v>116</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="66" t="s">
         <v>124</v>
       </c>
-      <c r="D16" s="68" t="s">
+      <c r="D16" s="67" t="s">
         <v>132</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="57" t="s">
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="L16" s="57" t="s">
+      <c r="L16" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="M16" s="57" t="s">
+      <c r="M16" s="56" t="s">
         <v>140</v>
       </c>
-      <c r="N16" s="57" t="s">
+      <c r="N16" s="56" t="s">
         <v>144</v>
       </c>
-      <c r="O16" s="57" t="s">
+      <c r="O16" s="56" t="s">
         <v>148</v>
       </c>
-      <c r="P16" s="57" t="s">
+      <c r="P16" s="56" t="s">
         <v>152</v>
       </c>
-      <c r="Q16" s="57" t="s">
+      <c r="Q16" s="56" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2495,40 +2518,40 @@
       <c r="A17" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="71" t="s">
+      <c r="B17" s="70" t="s">
         <v>117</v>
       </c>
-      <c r="C17" s="72" t="s">
+      <c r="C17" s="71" t="s">
         <v>125</v>
       </c>
-      <c r="D17" s="73" t="s">
+      <c r="D17" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="E17" s="74"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="76"/>
-      <c r="H17" s="76"/>
-      <c r="I17" s="76"/>
-      <c r="J17" s="76"/>
-      <c r="K17" s="58" t="s">
+      <c r="E17" s="73"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="75"/>
+      <c r="H17" s="75"/>
+      <c r="I17" s="75"/>
+      <c r="J17" s="75"/>
+      <c r="K17" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="L17" s="58" t="s">
+      <c r="L17" s="57" t="s">
         <v>137</v>
       </c>
-      <c r="M17" s="58" t="s">
+      <c r="M17" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="N17" s="58" t="s">
+      <c r="N17" s="57" t="s">
         <v>145</v>
       </c>
-      <c r="O17" s="58" t="s">
+      <c r="O17" s="57" t="s">
         <v>149</v>
       </c>
-      <c r="P17" s="58" t="s">
+      <c r="P17" s="57" t="s">
         <v>153</v>
       </c>
-      <c r="Q17" s="58" t="s">
+      <c r="Q17" s="57" t="s">
         <v>157</v>
       </c>
     </row>

</xml_diff>